<commit_message>
making example more realistic
</commit_message>
<xml_diff>
--- a/karr_lab_tutorials/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/karr_lab_tutorials/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,16 +22,26 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">submodels!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,18 +53,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="158">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
   <si>
-    <t xml:space="preserve">ASP_test_2016_2</t>
+    <t xml:space="preserve">wc_lang_tutorial_model</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">ASP test model 2</t>
+    <t xml:space="preserve">wc_lang tutorial model</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
@@ -69,13 +79,10 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">For wc_lang tutorial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASP_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test model for TestExecutableModel</t>
+    <t xml:space="preserve">mpn_m129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mycoplasma pneumoniae M129</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -84,10 +91,7 @@
     <t xml:space="preserve">Rank</t>
   </si>
   <si>
-    <t xml:space="preserve">domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rank not used</t>
+    <t xml:space="preserve">variety</t>
   </si>
   <si>
     <t xml:space="preserve">References</t>
@@ -96,7 +100,7 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
-    <t xml:space="preserve">submodel_1</t>
+    <t xml:space="preserve">metabolism</t>
   </si>
   <si>
     <t xml:space="preserve">Metabolism</t>
@@ -105,7 +109,7 @@
     <t xml:space="preserve">dfba</t>
   </si>
   <si>
-    <t xml:space="preserve">submodel_2</t>
+    <t xml:space="preserve">rna_degradation</t>
   </si>
   <si>
     <t xml:space="preserve">RNA degradation</t>
@@ -150,91 +154,138 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
+    <t xml:space="preserve">adp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADP(3-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/C10H15N5O10P2/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(24-10)1-23-27(21,22)25-26(18,19)20/h2-4,6-7,10,16-17H,1H2,(H,21,22)(H2,11,12,13)(H2,18,19,20)/p-3/t4-,6-,7-,10-/m1/s1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10H12N5O10P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metabolite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMP(2-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/C10H14N5O7P/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(22-10)1-21-23(18,19)20/h2-4,6-7,10,16-17H,1H2,(H2,11,12,13)(H2,18,19,20)/p-2/t4-,6-,7-,10-/m1/s1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10H12N5O7P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP(4-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/C10H16N5O13P3/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(26-10)1-25-30(21,22)28-31(23,24)27-29(18,19)20/h2-4,6-7,10,16-17H,1H2,(H,21,22)(H,23,24)(H2,11,12,13)(H2,18,19,20)/p-4/t4-,6-,7-,10-/m1/s1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10H12N5O13P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha-D-glucose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/C6H12O6/c7-1-2-3(8)4(9)5(10)6(11)12-2/h2-11H,1H2/t2-,3-,4+,5-,6+/m1/s1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6H12O6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/p+1/i/hH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/H2O/h1H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrogenphosphate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/H3O4P/c1-5(2,3)4/h(H3,1,2,3,4)/p-2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO4P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna_dec_a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA (A*10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAAAAAAAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C100H111N50O61P10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass</t>
   </si>
   <si>
     <t xml:space="preserve">pseudo_species</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2O2Na3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H3SO4C9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metabolite</t>
-  </si>
-  <si>
     <t xml:space="preserve">Species</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_1[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6[c]</t>
+    <t xml:space="preserve">adp[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atp[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pi[c]</t>
   </si>
   <si>
     <t xml:space="preserve">Submodel</t>
@@ -246,46 +297,40 @@
     <t xml:space="preserve">Reversible</t>
   </si>
   <si>
-    <t xml:space="preserve">reaction_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[c] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; biomass</t>
+    <t xml:space="preserve">atp_hydrolysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP hydrolysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: atp + h2o ==&gt; adp + pi + h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: atp + adp + pi + h2o + h ==&gt; biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glucose import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc[e] + atp[c] + h2o[c] ==&gt; glc[c] + adp[c] + pi[c] + h[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna_degradation_dec_a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA degradation (A*10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: rna_dec_a + (9) h2o ==&gt; (10) amp + (9) h</t>
   </si>
   <si>
     <t xml:space="preserve">Reaction</t>
@@ -303,22 +348,25 @@
     <t xml:space="preserve">K m</t>
   </si>
   <si>
+    <t xml:space="preserve">backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * atp[c] / (atp[c] + k_m)</t>
+  </si>
+  <si>
     <t xml:space="preserve">forward</t>
   </si>
   <si>
-    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c] / k_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+    <t xml:space="preserve">k_cat * adp[c] / (adp[c] + k_m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min( atp[c], adp[c] )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * glc[e] / (glc[e] + k_m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * rna_dec_a[c]</t>
   </si>
   <si>
     <t xml:space="preserve">Submodels</t>
@@ -336,7 +384,7 @@
     <t xml:space="preserve">dimensionless</t>
   </si>
   <si>
-    <t xml:space="preserve">[Ref-0006]</t>
+    <t xml:space="preserve">ref_0001</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
@@ -378,6 +426,42 @@
     <t xml:space="preserve">Pages</t>
   </si>
   <si>
+    <t xml:space="preserve">Hastings et al., 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChEBI in 2016: Improved services and an expanding collection of metabolites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hastings J, Owen G, Dekker A, Ennis M, Kale N, Muthukrishnan V, Turner S, Swainston N, Mendes P, Steinbeck C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nucleic Acids Res</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1214-D1210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref_0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benson et al., 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GenBank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benson DA, Cavanaugh M, Clark K, Karsch-Mizrachi I, Lipman DJ, Ostell J, Sayers EW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D37-D42</t>
+  </si>
+  <si>
     <t xml:space="preserve">Database</t>
   </si>
   <si>
@@ -397,6 +481,54 @@
   </si>
   <si>
     <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0008152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0006401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCO-CYTOPLASM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCO-EXTRACELLULAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chebi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:456215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:15377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:456216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:30616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:18367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:24636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rna</t>
   </si>
 </sst>
 </file>
@@ -507,7 +639,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -536,20 +668,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -560,7 +688,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -645,6 +773,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -655,13 +791,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -700,9 +836,6 @@
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -721,22 +854,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="30.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -748,52 +881,122 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -814,53 +1017,194 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>117</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>272634</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -884,22 +1228,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.1578947368421"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,12 +1251,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -920,23 +1264,20 @@
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -957,20 +1298,20 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="ALP2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="ALP1" activeCellId="0" sqref="ALP1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="ALP5" activeCellId="0" sqref="ALP5"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="3" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.7692307692308"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
@@ -984,44 +1325,44 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1047,15 +1388,16 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="43.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="44.1336032388664"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
   </cols>
@@ -1068,24 +1410,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1094,15 +1436,15 @@
         <v>4.58E-017</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
@@ -1111,7 +1453,7 @@
         <v>1E-012</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1132,30 +1474,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1163,191 +1505,255 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>424.1773</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>2</v>
+        <v>345.2053</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>38</v>
+        <v>-2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>3</v>
+        <v>45</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>503.14946</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>38</v>
+        <v>-4</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>4</v>
+        <v>180.15588</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>38</v>
+      <c r="H5" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>1.00783</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>6</v>
+        <v>18.0153</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>38</v>
+      <c r="H7" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F8" s="3" t="n">
-        <v>10</v>
+        <v>95.9793</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>55</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>3298.98577</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>-11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1368,14 +1774,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1384,77 +1790,86 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="3" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>0.000148</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="n">
-        <v>0.0002</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>0.0005</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>0.0005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>0.001</v>
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>1E-007</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>0.002</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1462,6 +1877,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1470,22 +1886,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="44.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1497,113 +1913,96 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>15</v>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>69</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>75</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="E4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="8" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D5"/>
@@ -1625,122 +2024,126 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.001</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>0.0003</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0.001</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.0003</v>
+        <v>2000</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E6" s="5" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="E6" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1748,6 +2151,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1763,18 +2167,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="42.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="6.31983805668016"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="47.4534412955466"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1785,30 +2190,30 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1817,10 +2222,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>97</v>
+        <v>108</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>